<commit_message>
ikut lelang terbuka (otomatis & manual)
</commit_message>
<xml_diff>
--- a/ikut lelang.xlsx
+++ b/ikut lelang.xlsx
@@ -11,15 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>jenis bid</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>batas_atas_penawaran</t>
+    <t>status_penawaran</t>
+  </si>
+  <si>
+    <t>harga_penawaran</t>
   </si>
   <si>
     <t>expected</t>
@@ -28,32 +28,32 @@
     <t>otomatis</t>
   </si>
   <si>
-    <t>deposit tidak mencukupi</t>
+    <t>kurang dari harga penawaran terakhir</t>
   </si>
   <si>
     <t>fail</t>
   </si>
   <si>
+    <t>sama dengan harga penawaran terakhir</t>
+  </si>
+  <si>
+    <t>lebih dari harga penawaran terakhir</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>kurang dari harga minimum</t>
+  </si>
+  <si>
     <t>manual</t>
-  </si>
-  <si>
-    <t>nominal = harga penawaran</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>nominal &lt; harga penawaran</t>
-  </si>
-  <si>
-    <t>nominal &gt; harga penawaran</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -63,6 +63,10 @@
       <b/>
     </font>
     <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -92,14 +96,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -318,7 +331,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="25.29"/>
+    <col customWidth="1" min="2" max="2" width="34.14"/>
     <col customWidth="1" min="3" max="3" width="22.86"/>
   </cols>
   <sheetData>
@@ -326,70 +339,126 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
-        <v>5.0E9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3">
+        <v>9.8E7</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3">
+        <v>9.85E7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>5.0E9</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" s="3">
+        <v>9.9E7</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
-        <v>5.0E9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="C5" s="3">
+        <v>7.0E7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.005E8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C7" s="3">
+        <v>2.0E9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
-        <v>5.0E9</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.005E9</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5.0E7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>